<commit_message>
Excel file added #3
</commit_message>
<xml_diff>
--- a/Author.xlsx
+++ b/Author.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Cspit-IT\3 Sem\SGP\004\Library management\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68F24FE3-9F1F-42C9-B766-04641ADA9FD5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B684CC2-691C-4BF6-AE86-6A1EF22291E9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1047" uniqueCount="876">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1049" uniqueCount="878">
   <si>
     <t>MOLLY CRABAPPLE</t>
   </si>
@@ -2650,12 +2650,19 @@
   </si>
   <si>
     <t>LAURIE HALSE ANDERSON</t>
+  </si>
+  <si>
+    <t>Mahatma Gandhi</t>
+  </si>
+  <si>
+    <t>Mohandas Karamchand Gandhi</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -3027,27 +3034,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J47" workbookViewId="0">
-      <selection activeCell="L70" sqref="L70"/>
+    <sheetView tabSelected="1" topLeftCell="I61" workbookViewId="0">
+      <selection activeCell="M70" sqref="M70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="34.6640625" customWidth="1"/>
-    <col min="2" max="2" width="30.44140625" customWidth="1"/>
-    <col min="3" max="3" width="27.33203125" customWidth="1"/>
-    <col min="4" max="4" width="40" customWidth="1"/>
-    <col min="5" max="5" width="27.33203125" customWidth="1"/>
-    <col min="6" max="6" width="27.44140625" customWidth="1"/>
-    <col min="7" max="7" width="35" customWidth="1"/>
-    <col min="8" max="8" width="118" customWidth="1"/>
-    <col min="9" max="9" width="28.44140625" customWidth="1"/>
-    <col min="10" max="10" width="27.44140625" customWidth="1"/>
-    <col min="11" max="11" width="30.33203125" customWidth="1"/>
-    <col min="12" max="12" width="27.5546875" customWidth="1"/>
-    <col min="13" max="13" width="28.109375" customWidth="1"/>
-    <col min="14" max="14" width="27.44140625" customWidth="1"/>
-    <col min="15" max="15" width="32.88671875" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="34.6640625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="30.44140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="27.33203125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="40.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="27.33203125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="27.44140625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="35.0" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="118.0" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="28.44140625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="27.44140625" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="30.33203125" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="27.5546875" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="28.109375" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="27.44140625" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="32.88671875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.3">
@@ -6329,6 +6336,9 @@
       </c>
       <c r="L70" t="s">
         <v>88</v>
+      </c>
+      <c r="M70" t="s">
+        <v>877</v>
       </c>
     </row>
   </sheetData>

</xml_diff>